<commit_message>
2021 Update and cleaning
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Pemaquid/Pemaquid August 2016/Pemaquid_Quad_Entry_2_1_17.xlsx
+++ b/raw_data/KEEN ONE/Pemaquid/Pemaquid August 2016/Pemaquid_Quad_Entry_2_1_17.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jebyrnes/Dropbox (Byrnes Lab)/Byrnes Lab Shared Folder/KEEN Data Processing/Monitoring/raw_data/KEEN ONE/Grabowski/2016/Pemaquid August 2016/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jebyrnes/Dropbox (Byrnes Lab)/Byrnes Lab Shared Folder/KEEN Data Processing/Monitoring/raw_data/KEEN ONE/Pemaquid/Pemaquid August 2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98D2FC1-5590-2F4A-B43D-66FF58F1FED1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F621599-7DD2-374E-9FB4-C0A2AA4C9612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="164">
   <si>
     <t>YEAR</t>
   </si>
@@ -266,157 +266,13 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>VALIDATION</t>
-  </si>
-  <si>
-    <t>AMS</t>
-  </si>
-  <si>
-    <t>ANAR</t>
-  </si>
-  <si>
-    <t>ANSP</t>
-  </si>
-  <si>
-    <t>BAEL</t>
-  </si>
-  <si>
     <t>BLD</t>
   </si>
   <si>
-    <t>CHOV</t>
-  </si>
-  <si>
-    <t>COCA</t>
-  </si>
-  <si>
-    <t>CUMI</t>
-  </si>
-  <si>
-    <t>CYJ</t>
-  </si>
-  <si>
-    <t>CYSP</t>
-  </si>
-  <si>
-    <t>DIOR</t>
-  </si>
-  <si>
-    <t>DIS</t>
-  </si>
-  <si>
-    <t>EAJ</t>
-  </si>
-  <si>
-    <t>EGJ</t>
-  </si>
-  <si>
-    <t>EUQU</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>LFJ</t>
-  </si>
-  <si>
-    <t>LIGS</t>
-  </si>
-  <si>
-    <t>MIID</t>
-  </si>
-  <si>
-    <t>NONO</t>
-  </si>
-  <si>
-    <t>OKS</t>
-  </si>
-  <si>
-    <t>OPES</t>
-  </si>
-  <si>
-    <t>OPSP</t>
-  </si>
-  <si>
-    <t>PACA</t>
-  </si>
-  <si>
-    <t>PAFI</t>
-  </si>
-  <si>
-    <t>PAST</t>
-  </si>
-  <si>
-    <t>PBS</t>
-  </si>
-  <si>
-    <t>PGS</t>
-  </si>
-  <si>
-    <t>PHS</t>
-  </si>
-  <si>
-    <t>POPL</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>PRUB</t>
-  </si>
-  <si>
-    <t>PTJ</t>
-  </si>
-  <si>
-    <t>PTTR</t>
-  </si>
-  <si>
-    <t>SFL</t>
-  </si>
-  <si>
-    <t>SFS</t>
-  </si>
-  <si>
-    <t>SKE</t>
-  </si>
-  <si>
-    <t>SPL</t>
-  </si>
-  <si>
-    <t>SPS</t>
-  </si>
-  <si>
-    <t>STMO</t>
-  </si>
-  <si>
-    <t>TEAU</t>
-  </si>
-  <si>
-    <t>TESP</t>
-  </si>
-  <si>
-    <t>URLO</t>
-  </si>
-  <si>
-    <t>URPI</t>
-  </si>
-  <si>
-    <t>PTL</t>
-  </si>
-  <si>
-    <t>CUSP</t>
-  </si>
-  <si>
-    <t>EUPO</t>
-  </si>
-  <si>
     <t>ENTERED BY</t>
   </si>
   <si>
     <t>CHECKED BY</t>
-  </si>
-  <si>
-    <t>MPJ</t>
   </si>
   <si>
     <t>DAY</t>
@@ -1524,7 +1380,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1533,9 +1389,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2089,11 +1942,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1048"/>
+  <dimension ref="A1:W220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2108,749 +1961,745 @@
     <col min="15" max="15" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
     <col min="17" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="14.5" customWidth="1"/>
+    <col min="18" max="19" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B2" s="37">
+        <v>8</v>
+      </c>
+      <c r="C2" s="36">
+        <v>3</v>
+      </c>
+      <c r="D2" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="36">
+        <v>3</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="36">
+        <v>2</v>
+      </c>
+      <c r="L2" s="36">
+        <v>1</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="37"/>
+      <c r="P2" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R2" s="36">
+        <v>8</v>
+      </c>
+      <c r="S2" s="36">
+        <v>10</v>
+      </c>
+      <c r="T2" s="36">
+        <v>5</v>
+      </c>
+      <c r="U2" s="36">
+        <v>16</v>
+      </c>
+      <c r="W2" s="37"/>
+    </row>
+    <row r="3" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B3" s="37">
+        <v>8</v>
+      </c>
+      <c r="C3" s="36">
+        <v>3</v>
+      </c>
+      <c r="D3" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="36">
+        <v>3</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="36">
+        <v>1</v>
+      </c>
+      <c r="I3" s="36">
+        <v>6</v>
+      </c>
+      <c r="J3" s="36">
+        <v>8</v>
+      </c>
+      <c r="K3" s="36">
+        <v>2</v>
+      </c>
+      <c r="L3" s="36">
+        <v>10</v>
+      </c>
+      <c r="M3" s="36">
+        <v>9</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="37"/>
+      <c r="P3" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R3" s="36">
+        <v>8</v>
+      </c>
+      <c r="S3" s="36">
+        <v>10</v>
+      </c>
+      <c r="T3" s="36">
+        <v>5</v>
+      </c>
+      <c r="U3" s="36">
+        <v>16</v>
+      </c>
+      <c r="W3" s="37"/>
+    </row>
+    <row r="4" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="37">
+        <v>8</v>
+      </c>
+      <c r="C4" s="36">
+        <v>3</v>
+      </c>
+      <c r="D4" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="36">
+        <v>3</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="36">
+        <v>3</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O4" s="37"/>
+      <c r="P4" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R4" s="36">
+        <v>8</v>
+      </c>
+      <c r="S4" s="36">
+        <v>10</v>
+      </c>
+      <c r="T4" s="36">
+        <v>5</v>
+      </c>
+      <c r="U4" s="36">
+        <v>16</v>
+      </c>
+      <c r="W4" s="37"/>
+    </row>
+    <row r="5" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="37">
+        <v>8</v>
+      </c>
+      <c r="C5" s="36">
+        <v>3</v>
+      </c>
+      <c r="D5" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="36">
+        <v>3</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="36">
+        <v>1</v>
+      </c>
+      <c r="I5" s="36">
+        <v>1</v>
+      </c>
+      <c r="J5" s="36">
+        <v>1</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O5" s="37"/>
+      <c r="P5" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R5" s="36">
+        <v>8</v>
+      </c>
+      <c r="S5" s="36">
+        <v>10</v>
+      </c>
+      <c r="T5" s="36">
+        <v>5</v>
+      </c>
+      <c r="U5" s="36">
+        <v>16</v>
+      </c>
+      <c r="W5" s="37"/>
+    </row>
+    <row r="6" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="37">
+        <v>8</v>
+      </c>
+      <c r="C6" s="36">
+        <v>3</v>
+      </c>
+      <c r="D6" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="36">
+        <v>3</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="I6" s="36">
+        <v>1</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O6" s="37"/>
+      <c r="P6" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R6" s="36">
+        <v>8</v>
+      </c>
+      <c r="S6" s="36">
+        <v>10</v>
+      </c>
+      <c r="T6" s="36">
+        <v>5</v>
+      </c>
+      <c r="U6" s="36">
+        <v>16</v>
+      </c>
+      <c r="W6" s="37"/>
+    </row>
+    <row r="7" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B7" s="37">
+        <v>8</v>
+      </c>
+      <c r="C7" s="36">
+        <v>3</v>
+      </c>
+      <c r="D7" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="36">
+        <v>3</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="36">
+        <v>1</v>
+      </c>
+      <c r="M7" s="36">
+        <v>1</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="36">
+        <v>8</v>
+      </c>
+      <c r="S7" s="36">
+        <v>10</v>
+      </c>
+      <c r="T7" s="36">
+        <v>5</v>
+      </c>
+      <c r="U7" s="36">
+        <v>16</v>
+      </c>
+      <c r="W7" s="37"/>
+    </row>
+    <row r="8" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="37">
+        <v>8</v>
+      </c>
+      <c r="C8" s="36">
+        <v>3</v>
+      </c>
+      <c r="D8" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="36">
+        <v>3</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="H8" s="36">
+        <v>2</v>
+      </c>
+      <c r="I8" s="36">
+        <v>2</v>
+      </c>
+      <c r="K8" s="36">
+        <v>4</v>
+      </c>
+      <c r="L8" s="36">
         <v>7</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="39" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="39">
+      <c r="M8" s="36">
+        <v>2</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="37"/>
+      <c r="P8" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="R8" s="36">
+        <v>8</v>
+      </c>
+      <c r="S8" s="36">
+        <v>10</v>
+      </c>
+      <c r="T8" s="36">
+        <v>5</v>
+      </c>
+      <c r="U8" s="36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="36">
         <v>2016</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B9" s="37">
         <v>8</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C9" s="36">
+        <v>8</v>
+      </c>
+      <c r="D9" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="36">
+        <v>4</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="36">
         <v>3</v>
       </c>
-      <c r="D2" s="41">
+      <c r="I9" s="36">
+        <v>4</v>
+      </c>
+      <c r="J9" s="36">
+        <v>6</v>
+      </c>
+      <c r="K9" s="36">
+        <v>4</v>
+      </c>
+      <c r="L9" s="36">
+        <v>8</v>
+      </c>
+      <c r="M9" s="36">
+        <v>9</v>
+      </c>
+      <c r="N9" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R9" s="36">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="S9" s="36">
+        <v>7.62</v>
+      </c>
+      <c r="T9" s="36">
+        <v>4</v>
+      </c>
+      <c r="U9" s="36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="37">
+        <v>8</v>
+      </c>
+      <c r="C10" s="36">
+        <v>8</v>
+      </c>
+      <c r="D10" s="38">
         <v>42767</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" s="39">
+      <c r="E10" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="36">
+        <v>4</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="I10" s="36">
         <v>3</v>
       </c>
-      <c r="G2" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="39">
+      <c r="J10" s="36">
+        <v>4</v>
+      </c>
+      <c r="K10" s="36">
+        <v>5</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R10" s="36">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="S10" s="36">
+        <v>7.62</v>
+      </c>
+      <c r="T10" s="36">
+        <v>4</v>
+      </c>
+      <c r="U10" s="36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B11" s="37">
+        <v>8</v>
+      </c>
+      <c r="C11" s="36">
+        <v>8</v>
+      </c>
+      <c r="D11" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="36">
+        <v>4</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="L11" s="36">
+        <v>1</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R11" s="36">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="S11" s="36">
+        <v>7.62</v>
+      </c>
+      <c r="T11" s="36">
+        <v>4</v>
+      </c>
+      <c r="U11" s="36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B12" s="37">
+        <v>8</v>
+      </c>
+      <c r="C12" s="36">
+        <v>8</v>
+      </c>
+      <c r="D12" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="36">
+        <v>4</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="36">
         <v>2</v>
       </c>
-      <c r="L2" s="39">
+      <c r="I12" s="36">
+        <v>2</v>
+      </c>
+      <c r="J12" s="36">
+        <v>3</v>
+      </c>
+      <c r="K12" s="36">
+        <v>2</v>
+      </c>
+      <c r="L12" s="36">
+        <v>5</v>
+      </c>
+      <c r="M12" s="36">
+        <v>5</v>
+      </c>
+      <c r="N12" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" s="36">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="S12" s="36">
+        <v>7.62</v>
+      </c>
+      <c r="T12" s="36">
+        <v>4</v>
+      </c>
+      <c r="U12" s="36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="36">
+        <v>2016</v>
+      </c>
+      <c r="B13" s="37">
+        <v>8</v>
+      </c>
+      <c r="C13" s="36">
+        <v>8</v>
+      </c>
+      <c r="D13" s="38">
+        <v>42767</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="36">
+        <v>4</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="H13" s="36">
         <v>1</v>
       </c>
-      <c r="N2" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O2" s="40"/>
-      <c r="P2" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S2" s="39">
-        <v>8</v>
-      </c>
-      <c r="T2" s="39">
-        <v>10</v>
-      </c>
-      <c r="U2" s="39">
-        <v>5</v>
-      </c>
-      <c r="V2" s="39">
-        <v>16</v>
-      </c>
-      <c r="X2" s="40"/>
-    </row>
-    <row r="3" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B3" s="40">
-        <v>8</v>
-      </c>
-      <c r="C3" s="39">
+      <c r="J13" s="36">
         <v>3</v>
       </c>
-      <c r="D3" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="39">
-        <v>3</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="H3" s="39">
-        <v>1</v>
-      </c>
-      <c r="I3" s="39">
-        <v>6</v>
-      </c>
-      <c r="J3" s="39">
-        <v>8</v>
-      </c>
-      <c r="K3" s="39">
-        <v>2</v>
-      </c>
-      <c r="L3" s="39">
-        <v>10</v>
-      </c>
-      <c r="M3" s="39">
-        <v>9</v>
-      </c>
-      <c r="N3" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" s="40"/>
-      <c r="P3" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S3" s="39">
-        <v>8</v>
-      </c>
-      <c r="T3" s="39">
-        <v>10</v>
-      </c>
-      <c r="U3" s="39">
-        <v>5</v>
-      </c>
-      <c r="V3" s="39">
-        <v>16</v>
-      </c>
-      <c r="X3" s="40"/>
-    </row>
-    <row r="4" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B4" s="40">
-        <v>8</v>
-      </c>
-      <c r="C4" s="39">
-        <v>3</v>
-      </c>
-      <c r="D4" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="39">
-        <v>3</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="39">
-        <v>3</v>
-      </c>
-      <c r="N4" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O4" s="40"/>
-      <c r="P4" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S4" s="39">
-        <v>8</v>
-      </c>
-      <c r="T4" s="39">
-        <v>10</v>
-      </c>
-      <c r="U4" s="39">
-        <v>5</v>
-      </c>
-      <c r="V4" s="39">
-        <v>16</v>
-      </c>
-      <c r="X4" s="40"/>
-    </row>
-    <row r="5" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B5" s="40">
-        <v>8</v>
-      </c>
-      <c r="C5" s="39">
-        <v>3</v>
-      </c>
-      <c r="D5" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="39">
-        <v>3</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="H5" s="39">
-        <v>1</v>
-      </c>
-      <c r="I5" s="39">
-        <v>1</v>
-      </c>
-      <c r="J5" s="39">
-        <v>1</v>
-      </c>
-      <c r="N5" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S5" s="39">
-        <v>8</v>
-      </c>
-      <c r="T5" s="39">
-        <v>10</v>
-      </c>
-      <c r="U5" s="39">
-        <v>5</v>
-      </c>
-      <c r="V5" s="39">
-        <v>16</v>
-      </c>
-      <c r="X5" s="40"/>
-    </row>
-    <row r="6" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B6" s="40">
-        <v>8</v>
-      </c>
-      <c r="C6" s="39">
-        <v>3</v>
-      </c>
-      <c r="D6" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="39">
-        <v>3</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>204</v>
-      </c>
-      <c r="I6" s="39">
-        <v>1</v>
-      </c>
-      <c r="N6" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O6" s="40"/>
-      <c r="P6" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S6" s="39">
-        <v>8</v>
-      </c>
-      <c r="T6" s="39">
-        <v>10</v>
-      </c>
-      <c r="U6" s="39">
-        <v>5</v>
-      </c>
-      <c r="V6" s="39">
-        <v>16</v>
-      </c>
-      <c r="X6" s="40"/>
-    </row>
-    <row r="7" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B7" s="40">
-        <v>8</v>
-      </c>
-      <c r="C7" s="39">
-        <v>3</v>
-      </c>
-      <c r="D7" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7" s="39">
-        <v>3</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="39">
-        <v>1</v>
-      </c>
-      <c r="M7" s="39">
-        <v>1</v>
-      </c>
-      <c r="N7" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S7" s="39">
-        <v>8</v>
-      </c>
-      <c r="T7" s="39">
-        <v>10</v>
-      </c>
-      <c r="U7" s="39">
-        <v>5</v>
-      </c>
-      <c r="V7" s="39">
-        <v>16</v>
-      </c>
-      <c r="X7" s="40"/>
-    </row>
-    <row r="8" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B8" s="40">
-        <v>8</v>
-      </c>
-      <c r="C8" s="39">
-        <v>3</v>
-      </c>
-      <c r="D8" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8" s="39">
-        <v>3</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="H8" s="39">
-        <v>2</v>
-      </c>
-      <c r="I8" s="39">
-        <v>2</v>
-      </c>
-      <c r="K8" s="39">
+      <c r="N13" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="R13" s="36">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="S13" s="36">
+        <v>7.62</v>
+      </c>
+      <c r="T13" s="36">
         <v>4</v>
       </c>
-      <c r="L8" s="39">
-        <v>7</v>
-      </c>
-      <c r="M8" s="39">
-        <v>2</v>
-      </c>
-      <c r="N8" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="S8" s="39">
-        <v>8</v>
-      </c>
-      <c r="T8" s="39">
-        <v>10</v>
-      </c>
-      <c r="U8" s="39">
-        <v>5</v>
-      </c>
-      <c r="V8" s="39">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B9" s="40">
-        <v>8</v>
-      </c>
-      <c r="C9" s="39">
-        <v>8</v>
-      </c>
-      <c r="D9" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="39">
-        <v>4</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="39">
-        <v>3</v>
-      </c>
-      <c r="I9" s="39">
-        <v>4</v>
-      </c>
-      <c r="J9" s="39">
-        <v>6</v>
-      </c>
-      <c r="K9" s="39">
-        <v>4</v>
-      </c>
-      <c r="L9" s="39">
-        <v>8</v>
-      </c>
-      <c r="M9" s="39">
-        <v>9</v>
-      </c>
-      <c r="N9" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="S9" s="39">
-        <v>4.8769999999999998</v>
-      </c>
-      <c r="T9" s="39">
-        <v>7.62</v>
-      </c>
-      <c r="U9" s="39">
-        <v>4</v>
-      </c>
-      <c r="V9" s="39">
+      <c r="U13" s="36">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B10" s="40">
-        <v>8</v>
-      </c>
-      <c r="C10" s="39">
-        <v>8</v>
-      </c>
-      <c r="D10" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="39">
-        <v>4</v>
-      </c>
-      <c r="G10" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="I10" s="39">
-        <v>3</v>
-      </c>
-      <c r="J10" s="39">
-        <v>4</v>
-      </c>
-      <c r="K10" s="39">
-        <v>5</v>
-      </c>
-      <c r="N10" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="S10" s="39">
-        <v>4.8769999999999998</v>
-      </c>
-      <c r="T10" s="39">
-        <v>7.62</v>
-      </c>
-      <c r="U10" s="39">
-        <v>4</v>
-      </c>
-      <c r="V10" s="39">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B11" s="40">
-        <v>8</v>
-      </c>
-      <c r="C11" s="39">
-        <v>8</v>
-      </c>
-      <c r="D11" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11" s="39">
-        <v>4</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="L11" s="39">
-        <v>1</v>
-      </c>
-      <c r="N11" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="S11" s="39">
-        <v>4.8769999999999998</v>
-      </c>
-      <c r="T11" s="39">
-        <v>7.62</v>
-      </c>
-      <c r="U11" s="39">
-        <v>4</v>
-      </c>
-      <c r="V11" s="39">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B12" s="40">
-        <v>8</v>
-      </c>
-      <c r="C12" s="39">
-        <v>8</v>
-      </c>
-      <c r="D12" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12" s="39">
-        <v>4</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12" s="39">
-        <v>2</v>
-      </c>
-      <c r="I12" s="39">
-        <v>2</v>
-      </c>
-      <c r="J12" s="39">
-        <v>3</v>
-      </c>
-      <c r="K12" s="39">
-        <v>2</v>
-      </c>
-      <c r="L12" s="39">
-        <v>5</v>
-      </c>
-      <c r="M12" s="39">
-        <v>5</v>
-      </c>
-      <c r="N12" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="S12" s="39">
-        <v>4.8769999999999998</v>
-      </c>
-      <c r="T12" s="39">
-        <v>7.62</v>
-      </c>
-      <c r="U12" s="39">
-        <v>4</v>
-      </c>
-      <c r="V12" s="39">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="39">
-        <v>2016</v>
-      </c>
-      <c r="B13" s="40">
-        <v>8</v>
-      </c>
-      <c r="C13" s="39">
-        <v>8</v>
-      </c>
-      <c r="D13" s="41">
-        <v>42767</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13" s="39">
-        <v>4</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="H13" s="39">
-        <v>1</v>
-      </c>
-      <c r="J13" s="39">
-        <v>3</v>
-      </c>
-      <c r="N13" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="S13" s="39">
-        <v>4.8769999999999998</v>
-      </c>
-      <c r="T13" s="39">
-        <v>7.62</v>
-      </c>
-      <c r="U13" s="39">
-        <v>4</v>
-      </c>
-      <c r="V13" s="39">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="G14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-    </row>
-    <row r="15" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="G15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-    </row>
-    <row r="16" spans="1:24" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="G16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-    </row>
-    <row r="17" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="G17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-    </row>
-    <row r="18" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="G18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-    </row>
-    <row r="19" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="G19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+    <row r="14" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="G14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+    </row>
+    <row r="15" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="G15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+    </row>
+    <row r="16" spans="1:23" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="G16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+    </row>
+    <row r="17" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="37"/>
+      <c r="D17" s="38"/>
+      <c r="G17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+    </row>
+    <row r="18" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="G18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+    </row>
+    <row r="19" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="G19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20"/>
@@ -5666,250 +5515,10 @@
       <c r="M220"/>
       <c r="N220"/>
     </row>
-    <row r="1001" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1001" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1002" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1002" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="1003" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1003" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1004" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1004" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="1005" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1005" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="1006" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1006" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1007" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1007" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1008" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1008" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1009" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1009" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="1010" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1010" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="1011" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1011" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="1012" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1012" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="1013" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1013" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="1014" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1014" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="1015" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1015" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="1016" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1016" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="1017" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1017" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="1018" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1018" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="1019" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1019" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="1020" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1020" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1021" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1021" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="1022" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1022" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="1023" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1023" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="1024" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1024" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="1025" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1025" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="1026" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1026" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="1027" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1027" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="1028" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1028" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="1029" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1029" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="1030" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1030" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="1031" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1031" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="1032" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1032" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="1033" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1033" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="1034" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1034" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="1035" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1035" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="1036" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1036" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="1037" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1037" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="1038" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1038" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="1039" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1039" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="1040" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1040" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="1041" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1041" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="1042" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1042" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="1043" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1043" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1044" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1044" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="1045" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1045" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="1046" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1046" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="1047" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1047" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="1048" spans="18:18" x14ac:dyDescent="0.15">
-      <c r="R1048" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,8,16,24,32,40"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B199:C65537" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -5920,7 +5529,7 @@
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W7" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"OFF, ON"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:M1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
@@ -5945,19 +5554,19 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>210</v>
+      <c r="A1" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="43">
+      <c r="A2" s="40">
         <v>43657</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>211</v>
+      <c r="B2" s="39" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5975,664 +5584,664 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="14" t="s">
-        <v>197</v>
+      <c r="B1" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="N5" s="17"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="N6" s="17"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="I7" s="14"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="I8" s="14"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="I15" s="14"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="I16" s="14"/>
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="I17" s="14"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="I18" s="14"/>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="28"/>
+      <c r="B25" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="29"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="14"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="28"/>
+      <c r="B38" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="14"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="14"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="14"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="14"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="24"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="22"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="16"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="16"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="16"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="16"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="16"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="15"/>
+      <c r="B60" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="15"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="15"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="15"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="15"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" s="15"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="15"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="31" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="B68" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="B69" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="N6" s="20"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18" t="s">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="I7" s="17"/>
-      <c r="N7" s="21"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="B73" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="34"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="I8" s="17"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="I9" s="17"/>
-      <c r="N9" s="22"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="B74" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" s="33"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="I11" s="25"/>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="B76" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="I12" s="17"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="B77" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="25"/>
+      <c r="B78" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="I15" s="17"/>
-      <c r="N15" s="26"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="I16" s="17"/>
-      <c r="N16" s="26"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="I17" s="17"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="I18" s="17"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="19"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
-      <c r="B21" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="N22" s="18"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
-      <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
-      <c r="B25" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="19"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="32"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="17"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="17"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="17"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
-      <c r="B38" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="17"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C40" s="19"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="17"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="17"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D45" s="17"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="27"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="D47" s="27"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="19"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C50" s="19"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" s="19"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="19"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C53" s="19"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C61" s="18"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C62" s="18"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="C63" s="18"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="C64" s="18"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="C66" s="18"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C67" s="18"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="25"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B73" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="C73" s="37"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C74" s="36"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B75" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" s="38"/>
-      <c r="D75" s="38"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B76" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C76" s="38"/>
-      <c r="D76" s="38"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="B77" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="28"/>
-      <c r="B78" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>